<commit_message>
feat: esquema exemplo para planilha de importação
</commit_message>
<xml_diff>
--- a/planilha-schema.xlsx
+++ b/planilha-schema.xlsx
@@ -6,7 +6,7 @@
     <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Folha1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Folha2" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <calcPr/>
   <extLst>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Nome</t>
   </si>
@@ -45,19 +45,7 @@
     <t xml:space="preserve">(82) 99999-9999</t>
   </si>
   <si>
-    <t xml:space="preserve">Serviço 1, Serviço 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Desafio 2</t>
-  </si>
-  <si>
-    <t>doity2@teste.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(82) 99999-9991</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Serviço 1</t>
+    <t xml:space="preserve">Design Figma</t>
   </si>
 </sst>
 </file>
@@ -98,8 +86,11 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
@@ -604,69 +595,48 @@
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
-  <cols>
-    <col bestFit="1" min="4" max="4" width="12.68359375"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" ht="14.25">
-      <c r="A1" t="s">
+    <row r="1">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" ht="14.25">
+    <row r="2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="3" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="3" ht="14.25">
-      <c r="A3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="C2"/>
-    <hyperlink r:id="rId2" ref="C3"/>
   </hyperlinks>
   <printOptions headings="0" gridLines="0"/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157500000008" bottom="0.78740157500000008" header="0.31496062000000008" footer="0.31496062000000008"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>

</xml_diff>